<commit_message>
fout eruit gehaald die ervoor zorgde dat opvragen van de voorspellingen bij een url die niet in het model zit een exception geeft
</commit_message>
<xml_diff>
--- a/Experiments/Experiments.xlsx
+++ b/Experiments/Experiments.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>ML experiments</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve">Result without same domain: </t>
+  </si>
+  <si>
+    <t>Distance</t>
   </si>
 </sst>
 </file>
@@ -431,10 +434,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -443,12 +446,12 @@
     <col min="2" max="2" width="27.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C4">
         <v>1</v>
       </c>
@@ -461,36 +464,42 @@
       <c r="F4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="D5">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+      <c r="G5">
+        <v>3.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F6">
         <v>52</v>

</xml_diff>